<commit_message>
data import and cleaning finished
</commit_message>
<xml_diff>
--- a/Project 2/data_sets/arrival_14.xlsx
+++ b/Project 2/data_sets/arrival_14.xlsx
@@ -14,7 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Time</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30,7 +34,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -62,13 +66,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="21" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -372,113 +379,118 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="17.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1">
-        <v>1.5216319444444446</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1">
-        <v>1.5216435185185184</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1">
-        <v>1.5220717592592594</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1">
-        <v>1.5228356481481482</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1">
-        <v>1.5230555555555556</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="1">
-        <v>1.5231944444444445</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="1">
-        <v>1.5235069444444445</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="1">
-        <v>1.5235300925925928</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="1">
-        <v>1.525162037037037</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="1">
-        <v>1.5253703703703705</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="1">
-        <v>1.528912037037037</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="1">
-        <v>1.5290856481481483</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="1">
-        <v>1.5303819444444444</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1">
-        <v>1.5304398148148148</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1">
-        <v>1.5304861111111112</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1">
-        <v>1.5336226851851853</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1">
-        <v>1.5341087962962963</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1">
-        <v>1.5344328703703702</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1">
-        <v>1.5347685185185185</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1">
-        <v>1.5348958333333333</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="2">
+        <v>2.5216319444444446</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="2">
+        <v>2.5216435185185184</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="2">
+        <v>2.5220717592592594</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="2">
+        <v>2.522835648148148</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="2">
+        <v>2.5230555555555556</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="2">
+        <v>2.5231944444444445</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="2">
+        <v>2.5235069444444447</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="2">
+        <v>2.5235300925925923</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="2">
+        <v>2.5251620370370373</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="2">
+        <v>2.5253703703703705</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="2">
+        <v>2.528912037037037</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="2">
+        <v>2.529085648148148</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="2">
+        <v>2.5303819444444446</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="2">
+        <v>2.530439814814815</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="2">
+        <v>2.530486111111111</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="2">
+        <v>2.5336226851851853</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="2">
+        <v>2.5341087962962963</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="2">
+        <v>2.5344328703703702</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="2">
+        <v>2.5347685185185185</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+      <c r="A21" s="2">
+        <v>2.5348958333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>